<commit_message>
updating link to drone modes
</commit_message>
<xml_diff>
--- a/Trajecotry/Autonomous/simulation/UBC/comparison_differentWinds/different wind.xlsx
+++ b/Trajecotry/Autonomous/simulation/UBC/comparison_differentWinds/different wind.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>index</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pitch_10N </t>
+  </si>
+  <si>
+    <t>average</t>
   </si>
 </sst>
 </file>
@@ -11957,15 +11960,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11987,15 +11990,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>823912</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>233362</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12017,15 +12020,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>519112</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>728662</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>52387</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12047,15 +12050,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>185737</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>623887</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>747712</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12077,15 +12080,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>719176</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>108378</xdr:rowOff>
+      <xdr:colOff>843001</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>165528</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>242926</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>184578</xdr:rowOff>
+      <xdr:colOff>366751</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>51228</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12107,15 +12110,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>369093</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>58184</xdr:rowOff>
+      <xdr:colOff>492918</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>115334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>654843</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>134384</xdr:rowOff>
+      <xdr:colOff>778668</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>1034</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12137,15 +12140,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>276550</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:colOff>400375</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12169,7 +12172,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5715325" y="20259674"/>
+          <a:off x="5839150" y="22602824"/>
           <a:ext cx="3457249" cy="2619375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -12455,15 +12458,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF74"/>
+  <dimension ref="A1:AF75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O115" sqref="O115"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -18195,6 +18198,43 @@
         <v>-13.1300001144409</v>
       </c>
     </row>
+    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75">
+        <f>AVERAGE(B2:B74)</f>
+        <v>114.97054896942502</v>
+      </c>
+      <c r="E75">
+        <f t="shared" ref="C75:O75" si="0">AVERAGE(E2:E74)</f>
+        <v>122.22862985689311</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="0"/>
+        <v>114.97383546175965</v>
+      </c>
+      <c r="M75">
+        <f t="shared" si="0"/>
+        <v>122.44547940606908</v>
+      </c>
+      <c r="R75">
+        <f t="shared" ref="R75" si="1">AVERAGE(R2:R74)</f>
+        <v>114.97383546175965</v>
+      </c>
+      <c r="U75">
+        <f t="shared" ref="U75" si="2">AVERAGE(U2:U74)</f>
+        <v>122.44547940606908</v>
+      </c>
+      <c r="Z75">
+        <f t="shared" ref="Z75" si="3">AVERAGE(Z2:Z74)</f>
+        <v>114.96411101458774</v>
+      </c>
+      <c r="AC75">
+        <f t="shared" ref="AC75" si="4">AVERAGE(AC2:AC74)</f>
+        <v>122.23273948773914</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>